<commit_message>
updated the demo project to include genre
</commit_message>
<xml_diff>
--- a/sample/SSIS/data/Films.xlsx
+++ b/sample/SSIS/data/Films.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Public\SsisUp\sample\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Public\SsisUp\sample\SSIS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -32,23 +32,66 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Matrix</t>
-  </si>
-  <si>
-    <t>Rocky</t>
+    <t>Genre</t>
+  </si>
+  <si>
+    <t>Batman - The Dark Knight</t>
+  </si>
+  <si>
+    <t>Fantasy</t>
+  </si>
+  <si>
+    <t>Batman Begins</t>
+  </si>
+  <si>
+    <t>Cars</t>
+  </si>
+  <si>
+    <t>Animation</t>
+  </si>
+  <si>
+    <t>Cars 2</t>
+  </si>
+  <si>
+    <t>City of God</t>
+  </si>
+  <si>
+    <t>Drama</t>
+  </si>
+  <si>
+    <t>Cool Runnings</t>
+  </si>
+  <si>
+    <t>Comedy</t>
+  </si>
+  <si>
+    <t>Fast and the Furious</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Iron Man</t>
+  </si>
+  <si>
+    <t>Monty Python's Life of Brian</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -68,14 +111,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -353,36 +398,127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>1999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>1978</v>
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>1993</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>1979</v>
       </c>
     </row>
   </sheetData>

</xml_diff>